<commit_message>
test(#56): download 2nd round format
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/2차전형점수.xlsx
+++ b/src/test/resources/xlsx/2차전형점수.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gimhanul/maru/src/test/resources/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7502A33-341F-A545-BB9F-A7EF42650331}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45FF5010-9BBF-974A-A7C6-3C5FFE2E8227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{7690012B-BFFA-3C48-824D-509550F219F4}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17800" xr2:uid="{7690012B-BFFA-3C48-824D-509550F219F4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="&quot;₩&quot;#,##0"/>
+    <numFmt numFmtId="176" formatCode="&quot;₩&quot;#,##0"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -154,7 +154,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -474,13 +474,13 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A35" sqref="A6:XFD35"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
   <cols>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>